<commit_message>
updated for over/underlimit changes
</commit_message>
<xml_diff>
--- a/ftest/data/fm29/Worked example policy calculation_Max deductibles.xlsx
+++ b/ftest/data/fm29/Worked example policy calculation_Max deductibles.xlsx
@@ -1,22 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm8\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\ktest_new\ftest\data\fm29\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3ECE7D16-FB62-4B50-B426-61DE0405D5C8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8EA0811-DADA-442E-934B-5EC922C7537C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2616" yWindow="0" windowWidth="14340" windowHeight="9348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worked examples" sheetId="10" r:id="rId1"/>
     <sheet name="Oasis Implementation" sheetId="8" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -843,14 +850,14 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1266,8 +1273,8 @@
   </sheetPr>
   <dimension ref="A1:N45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1445,18 +1452,18 @@
       <c r="B10" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="70">
+      <c r="C10" s="71">
         <v>0.05</v>
       </c>
-      <c r="D10" s="70"/>
-      <c r="E10" s="70"/>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70">
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="71">
         <v>0.05</v>
       </c>
-      <c r="H10" s="70"/>
-      <c r="I10" s="70"/>
-      <c r="J10" s="70"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="71"/>
+      <c r="J10" s="71"/>
       <c r="K10" s="36"/>
       <c r="L10" s="43"/>
     </row>
@@ -1696,20 +1703,20 @@
       <c r="B21" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="71">
+      <c r="C21" s="72">
         <f>SUM(C9:F9)*C10</f>
         <v>58500</v>
       </c>
-      <c r="D21" s="71"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="71"/>
-      <c r="G21" s="71">
+      <c r="D21" s="72"/>
+      <c r="E21" s="72"/>
+      <c r="F21" s="72"/>
+      <c r="G21" s="72">
         <f>SUM(G9:J9)*G10</f>
         <v>58500</v>
       </c>
-      <c r="H21" s="71"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="71"/>
+      <c r="H21" s="72"/>
+      <c r="I21" s="72"/>
+      <c r="J21" s="72"/>
       <c r="K21" s="58"/>
       <c r="L21" s="59"/>
     </row>
@@ -1720,20 +1727,20 @@
       <c r="B22" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="C22" s="72">
+      <c r="C22" s="70">
         <f>SUM(C20:F20)</f>
         <v>112900</v>
       </c>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72">
+      <c r="D22" s="70"/>
+      <c r="E22" s="70"/>
+      <c r="F22" s="70"/>
+      <c r="G22" s="70">
         <f>SUM(G20:J20)</f>
         <v>10000</v>
       </c>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
+      <c r="H22" s="70"/>
+      <c r="I22" s="70"/>
+      <c r="J22" s="70"/>
       <c r="K22" s="57"/>
       <c r="L22" s="42"/>
     </row>
@@ -1744,46 +1751,49 @@
       <c r="B23" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="C23" s="72">
+      <c r="C23" s="70">
         <f>MIN(C22,C21)</f>
         <v>58500</v>
       </c>
-      <c r="D23" s="72"/>
-      <c r="E23" s="72"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="72">
+      <c r="D23" s="70"/>
+      <c r="E23" s="70"/>
+      <c r="F23" s="70"/>
+      <c r="G23" s="70">
         <f>MIN(G22,G21)</f>
         <v>10000</v>
       </c>
-      <c r="H23" s="72"/>
-      <c r="I23" s="72"/>
-      <c r="J23" s="72"/>
+      <c r="H23" s="70"/>
+      <c r="I23" s="70"/>
+      <c r="J23" s="70"/>
       <c r="K23" s="60"/>
       <c r="L23" s="61">
         <f>SUM(C23:J23)</f>
         <v>68500</v>
       </c>
-      <c r="M23" s="62"/>
+      <c r="M23" s="62">
+        <f>L24+L23-L25</f>
+        <v>82900</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" s="38" t="s">
         <v>105</v>
       </c>
       <c r="B24" s="39"/>
-      <c r="C24" s="72">
+      <c r="C24" s="70">
         <f>C22-C23</f>
         <v>54400</v>
       </c>
-      <c r="D24" s="72"/>
-      <c r="E24" s="72"/>
-      <c r="F24" s="72"/>
-      <c r="G24" s="72">
+      <c r="D24" s="70"/>
+      <c r="E24" s="70"/>
+      <c r="F24" s="70"/>
+      <c r="G24" s="70">
         <f>G22-G23</f>
         <v>0</v>
       </c>
-      <c r="H24" s="72"/>
-      <c r="I24" s="72"/>
-      <c r="J24" s="72"/>
+      <c r="H24" s="70"/>
+      <c r="I24" s="70"/>
+      <c r="J24" s="70"/>
       <c r="K24" s="60"/>
       <c r="L24" s="61">
         <f>SUM(C24:J24)</f>

</xml_diff>